<commit_message>
testplan + logical topology extended
</commit_message>
<xml_diff>
--- a/teszteles.xlsx
+++ b/teszteles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bence\Documents\GitHub\oprendszerek_beadando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241A25E-A8D1-4111-BAFD-34509CB5AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C5A00D-8B6A-4626-BAE7-F68191AA43FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-120" windowWidth="27900" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14970" yWindow="0" windowWidth="13830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>Elvárt eredmény</t>
   </si>
@@ -34,22 +34,164 @@
 (mit teszteltünk)</t>
   </si>
   <si>
-    <t>Tesztelés módja 
-(miként teszteltük)</t>
-  </si>
-  <si>
-    <t>Tesztelés végrehajtója 
-(kivel teszteljük)</t>
+    <t>Sikeres</t>
+  </si>
+  <si>
+    <t>Teszt azonosító</t>
+  </si>
+  <si>
+    <t>NET_01</t>
+  </si>
+  <si>
+    <t>NET_02</t>
+  </si>
+  <si>
+    <t>NET_03</t>
+  </si>
+  <si>
+    <t>NET_04</t>
+  </si>
+  <si>
+    <t>NET_05</t>
+  </si>
+  <si>
+    <t>NET_06</t>
+  </si>
+  <si>
+    <t>NET_07</t>
+  </si>
+  <si>
+    <t>NET_08</t>
+  </si>
+  <si>
+    <t>NET_09</t>
+  </si>
+  <si>
+    <t>NET_10</t>
+  </si>
+  <si>
+    <t>NET_11</t>
+  </si>
+  <si>
+    <t>NET_12</t>
+  </si>
+  <si>
+    <t>NET_13</t>
+  </si>
+  <si>
+    <t>NET_14</t>
+  </si>
+  <si>
+    <t>NET_15</t>
+  </si>
+  <si>
+    <t>NET_16</t>
+  </si>
+  <si>
+    <t>NET_17</t>
+  </si>
+  <si>
+    <t>NET_18</t>
+  </si>
+  <si>
+    <t>NET_19</t>
+  </si>
+  <si>
+    <t>NET_20</t>
+  </si>
+  <si>
+    <t>Router elérése WinBoxban</t>
+  </si>
+  <si>
+    <t>Router konfigurációs felületének elérése 80-as porton keresztül</t>
+  </si>
+  <si>
+    <t>Sikertelen</t>
+  </si>
+  <si>
+    <t>Router elérése Telnettel</t>
+  </si>
+  <si>
+    <t>Router elérése SSH-val</t>
+  </si>
+  <si>
+    <t>Router elérése SSH-val 22-es porton keresztül</t>
+  </si>
+  <si>
+    <t>Router elérése SSH-val a beállított porton keresztül</t>
+  </si>
+  <si>
+    <t>Router konfigurációs felületének elérése a beállított porton keresztül</t>
+  </si>
+  <si>
+    <t>Routerre fájlokat juttatunk FTP protokoll segítségével</t>
+  </si>
+  <si>
+    <t>Webszerver elérése SSH-val a routeren keresztül (port forwarding)</t>
+  </si>
+  <si>
+    <t>Iskola honlapjának elérése a routeren (gatewayen) keresztül (port forwarding)</t>
+  </si>
+  <si>
+    <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>elrontott portkonfigokat vissza tudjuk hozni Winboxban</t>
+  </si>
+  <si>
+    <t>hardeninget teszteljük</t>
+  </si>
+  <si>
+    <t>DHCP-szerver konfigurációját teszteljük</t>
+  </si>
+  <si>
+    <t>tűzfalbeállításokat teszteljük</t>
+  </si>
+  <si>
+    <t>webszerver 10.0.0.2 címet kapja DHCP-szervertől</t>
+  </si>
+  <si>
+    <t>DHCP-vel IP-konfigurációk kiosztása egy újabb, 30. gép részére</t>
+  </si>
+  <si>
+    <t>DHCP-vel IP-konfigurációk kiosztása 29 géptermi gép részére</t>
+  </si>
+  <si>
+    <t>gepterem1 és gepterem2 gépei elérik egymást (ping)</t>
+  </si>
+  <si>
+    <t>az Internal belső hálózat gépei a 10.0.0.2-31 tartományból kapnak címeket</t>
+  </si>
+  <si>
+    <t>Internal és gepterem1 gépei elérik egymást (ping)</t>
+  </si>
+  <si>
+    <t>gepterem2 és gepterem3 gépei elérik egymást (ping)</t>
+  </si>
+  <si>
+    <t>a gepterem1 belső hálózat gépei a 10.0.0.34-62 tartományból kapnak címeket</t>
+  </si>
+  <si>
+    <t>a gepterem2 belső hálózat gépei a 10.0.0.66-94 tartományból kapnak címeket</t>
+  </si>
+  <si>
+    <t>a gepterem3 belső hálózat gépei a 10.0.0.98-126 tartományból kapnak címeket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +217,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -363,35 +508,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D21" sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>